<commit_message>
adding spreadsheets with cohort analysis
</commit_message>
<xml_diff>
--- a/notebooks/df3.xlsx
+++ b/notebooks/df3.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erinm\Documents\donations\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{411240B3-C7A2-418F-8960-D861BD82275B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5744BA7A-44BB-4113-A86C-7742A6BD7E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="df3" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="206">
   <si>
     <t>cohort_year</t>
   </si>
@@ -634,130 +643,27 @@
     <t>0001107b9faa5c3bb42cfcecece1d587</t>
   </si>
   <si>
-    <t>#giving</t>
-  </si>
-  <si>
-    <t>patterns</t>
-  </si>
-  <si>
-    <t>&gt;0)</t>
-  </si>
-  <si>
-    <t>&amp;</t>
-  </si>
-  <si>
-    <t>==0)</t>
-  </si>
-  <si>
-    <t>0)</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>choices</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>['0,',</t>
-  </si>
-  <si>
-    <t>'0,1,',</t>
-  </si>
-  <si>
-    <t>'0,2,',</t>
-  </si>
-  <si>
-    <t>'0,3,',</t>
-  </si>
-  <si>
-    <t>'0,4,',</t>
-  </si>
-  <si>
-    <t>'0,1,2,',</t>
-  </si>
-  <si>
-    <t>'0,1,3,',</t>
-  </si>
-  <si>
-    <t>'0,1,4,',</t>
-  </si>
-  <si>
-    <t>'0,2,3,',</t>
-  </si>
-  <si>
-    <t>'0,2,4,',</t>
-  </si>
-  <si>
-    <t>'0,3,4',</t>
-  </si>
-  <si>
-    <t>'0,1,2,3,',</t>
-  </si>
-  <si>
-    <t>'0,1,2,4,',</t>
-  </si>
-  <si>
-    <t>'0,1,3,4,',</t>
-  </si>
-  <si>
-    <t>'0,2,3,4,',</t>
-  </si>
-  <si>
-    <t>'0,1,2,3,4,']</t>
-  </si>
-  <si>
-    <t>np.select(conditions,</t>
-  </si>
-  <si>
-    <t>choices,</t>
-  </si>
-  <si>
-    <t>default='none')</t>
-  </si>
-  <si>
-    <t>conditions=[(donations[('amount_yr0')]</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr1')]</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr2')]==0)</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr3')]==0)</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr4')]==</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr0')]</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr2')]&gt;0)</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr3')]&gt;0)</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr4')]&gt;</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr4')]&gt;0)</t>
-  </si>
-  <si>
-    <t>(donations[('amount_yr4')]&gt;0)]</t>
-  </si>
-  <si>
-    <t>donations.loc[:,'cohort_gift_pattern']</t>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>ERIN</t>
+  </si>
+  <si>
+    <t>PETE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="0.000000000000"/>
+    <numFmt numFmtId="178" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="179" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="180" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="181" formatCode="0.00000000000000000"/>
+    <numFmt numFmtId="184" formatCode="0.00000000000000000000"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1242,11 +1148,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1367,26 +1279,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1457,6 +1349,26 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1471,8 +1383,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B188" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
-  <autoFilter ref="A1:B188">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:B188" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:B188" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="1">
       <customFilters>
         <customFilter operator="notEqual" val="0"/>
@@ -1480,16 +1392,16 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Column1" dataDxfId="9"/>
-    <tableColumn id="2" name="Column2" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B188" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:B188">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:B188" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B188" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="1">
       <customFilters>
         <customFilter operator="greaterThan" val="0"/>
@@ -1497,8 +1409,8 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" name="Column2" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1800,11 +1712,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1812,16 +1724,16 @@
     <col min="1" max="1" width="1.68359375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.62890625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.62890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.3125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7890625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26171875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7890625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.1015625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.5234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.47265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.26171875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.9453125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.20703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.89453125" bestFit="1" customWidth="1"/>
@@ -1830,7 +1742,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1895,7 +1807,7 @@
         <v>33</v>
       </c>
       <c r="F2">
-        <v>164.2114</v>
+        <v>497.61030303030299</v>
       </c>
       <c r="G2">
         <v>76.595744680850999</v>
@@ -1907,7 +1819,7 @@
         <v>12</v>
       </c>
       <c r="J2">
-        <v>192.3141</v>
+        <v>1597.2608333333301</v>
       </c>
       <c r="K2">
         <v>63.636363636363598</v>
@@ -1922,7 +1834,7 @@
         <v>2</v>
       </c>
       <c r="O2">
-        <v>192.3141</v>
+        <v>32.14</v>
       </c>
       <c r="P2">
         <v>98.148148148148096</v>
@@ -1948,7 +1860,7 @@
         <v>62130</v>
       </c>
       <c r="F3">
-        <v>152677.0398</v>
+        <v>245.73803283437999</v>
       </c>
       <c r="G3">
         <v>80.588560591622397</v>
@@ -1960,7 +1872,7 @@
         <v>26080</v>
       </c>
       <c r="J3">
-        <v>125873.073900002</v>
+        <v>407.96834739264398</v>
       </c>
       <c r="K3">
         <v>58.023499114759304</v>
@@ -1975,7 +1887,7 @@
         <v>16153</v>
       </c>
       <c r="O3">
-        <v>125873.073900002</v>
+        <v>120.56539899709</v>
       </c>
       <c r="P3">
         <v>93.737666657620593</v>
@@ -2001,7 +1913,7 @@
         <v>48667</v>
       </c>
       <c r="F4">
-        <v>77458.972600003501</v>
+        <v>159.16118232067601</v>
       </c>
       <c r="G4">
         <v>84.823480617326595</v>
@@ -2013,7 +1925,7 @@
         <v>15739</v>
       </c>
       <c r="J4">
-        <v>64377.087699999698</v>
+        <v>299.721816506766</v>
       </c>
       <c r="K4">
         <v>67.659810549242806</v>
@@ -2028,7 +1940,7 @@
         <v>15786</v>
       </c>
       <c r="O4">
-        <v>64377.087699999698</v>
+        <v>108.98182566831299</v>
       </c>
       <c r="P4">
         <v>94.196451548862896</v>
@@ -2054,7 +1966,7 @@
         <v>46078</v>
       </c>
       <c r="F5">
-        <v>82805.4987000002</v>
+        <v>179.707232735796</v>
       </c>
       <c r="G5">
         <v>87.025288832197106</v>
@@ -2066,7 +1978,7 @@
         <v>15323</v>
       </c>
       <c r="J5">
-        <v>74441.456300000005</v>
+        <v>366.02032173856298</v>
       </c>
       <c r="K5">
         <v>66.7455184686835</v>
@@ -2081,7 +1993,7 @@
         <v>16520</v>
       </c>
       <c r="O5">
-        <v>74441.456300000005</v>
+        <v>111.11478450363199</v>
       </c>
       <c r="P5">
         <v>94.654742298396101</v>
@@ -2107,7 +2019,7 @@
         <v>56538</v>
       </c>
       <c r="F6">
-        <v>104757.6027</v>
+        <v>185.287068343415</v>
       </c>
       <c r="G6">
         <v>87.3118820102424</v>
@@ -2119,7 +2031,7 @@
         <v>10335</v>
       </c>
       <c r="J6">
-        <v>28855.4002</v>
+        <v>205.31895500725599</v>
       </c>
       <c r="K6">
         <v>81.718490218967702</v>
@@ -2134,7 +2046,7 @@
         <v>8338</v>
       </c>
       <c r="O6">
-        <v>28855.4002</v>
+        <v>91.576951307267805</v>
       </c>
       <c r="P6">
         <v>97.856628797614704</v>
@@ -2160,7 +2072,7 @@
         <v>29990</v>
       </c>
       <c r="F7">
-        <v>45499.131999999998</v>
+        <v>151.71434478159401</v>
       </c>
       <c r="G7">
         <v>93.105604483770904</v>
@@ -2224,7 +2136,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>205</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -2663,7 +2575,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>333.39890303030302</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
@@ -2679,7 +2591,7 @@
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>1404.94673333333</v>
+        <v>0</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
@@ -2699,7 +2611,7 @@
       </c>
       <c r="O20">
         <f t="shared" si="0"/>
-        <v>-160.17410000000001</v>
+        <v>0</v>
       </c>
       <c r="P20">
         <f t="shared" si="0"/>
@@ -2719,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f>D12-D3</f>
         <v>9.9475983006414026E-14</v>
       </c>
       <c r="E21">
@@ -2728,7 +2640,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>-152431.30176716563</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
@@ -2744,7 +2656,7 @@
       </c>
       <c r="J21">
         <f t="shared" si="1"/>
-        <v>-125465.10555260936</v>
+        <v>-5.9685589803848416E-12</v>
       </c>
       <c r="K21">
         <f t="shared" si="1"/>
@@ -2764,7 +2676,7 @@
       </c>
       <c r="O21">
         <f t="shared" si="1"/>
-        <v>-125752.50850100491</v>
+        <v>0</v>
       </c>
       <c r="P21">
         <f t="shared" si="1"/>
@@ -2793,7 +2705,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>-77299.811417682839</v>
+        <v>-6.9917405198793858E-12</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
@@ -2809,7 +2721,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="1"/>
-        <v>-64077.36588349293</v>
+        <v>1.0231815394945443E-12</v>
       </c>
       <c r="K22">
         <f t="shared" si="1"/>
@@ -2829,7 +2741,7 @@
       </c>
       <c r="O22">
         <f t="shared" si="1"/>
-        <v>-64268.105874331384</v>
+        <v>1.0089706847793423E-12</v>
       </c>
       <c r="P22">
         <f t="shared" si="1"/>
@@ -2858,7 +2770,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>-82625.791467264411</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
@@ -2874,7 +2786,7 @@
       </c>
       <c r="J23">
         <f t="shared" si="1"/>
-        <v>-74075.435978261448</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <f t="shared" si="1"/>
@@ -2894,7 +2806,7 @@
       </c>
       <c r="O23">
         <f t="shared" si="1"/>
-        <v>-74330.341515496373</v>
+        <v>0</v>
       </c>
       <c r="P23">
         <f t="shared" si="1"/>
@@ -2923,7 +2835,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>-104572.31563165659</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
@@ -2939,7 +2851,7 @@
       </c>
       <c r="J24">
         <f t="shared" si="1"/>
-        <v>-28650.081244992743</v>
+        <v>9.9475983006414026E-13</v>
       </c>
       <c r="K24">
         <f t="shared" si="1"/>
@@ -2959,7 +2871,7 @@
       </c>
       <c r="O24">
         <f t="shared" si="1"/>
-        <v>-28763.823248692734</v>
+        <v>0</v>
       </c>
       <c r="P24">
         <f t="shared" si="1"/>
@@ -2988,7 +2900,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>-45347.417655218407</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
@@ -3105,7 +3017,7 @@
         <f>SUM(C20:C26)</f>
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="8">
         <f t="shared" ref="D28:Q28" si="2">SUM(D20:D26)</f>
         <v>2.007283228522283E-13</v>
       </c>
@@ -3113,15 +3025,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="4">
         <f t="shared" si="2"/>
-        <v>-461943.23903595761</v>
+        <v>-6.9917405198793858E-12</v>
       </c>
       <c r="G28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="6">
         <f t="shared" si="2"/>
         <v>4.0145664570445661E-13</v>
       </c>
@@ -3129,11 +3041,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="4">
         <f t="shared" si="2"/>
-        <v>-290863.04192602314</v>
-      </c>
-      <c r="K28">
+        <v>-3.950617610826157E-12</v>
+      </c>
+      <c r="K28" s="5">
         <f t="shared" si="2"/>
         <v>9.9475983006414026E-14</v>
       </c>
@@ -3141,7 +3053,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="7">
         <f t="shared" si="2"/>
         <v>1.9539925233402755E-14</v>
       </c>
@@ -3149,9 +3061,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="4">
         <f t="shared" si="2"/>
-        <v>-293274.95323952538</v>
+        <v>1.0089706847793423E-12</v>
       </c>
       <c r="P28">
         <f t="shared" si="2"/>
@@ -3162,12 +3074,59 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29" t="s">
+        <v>203</v>
+      </c>
+      <c r="E29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F29" t="s">
+        <v>203</v>
+      </c>
+      <c r="G29" t="s">
+        <v>203</v>
+      </c>
+      <c r="H29" t="s">
+        <v>203</v>
+      </c>
+      <c r="I29" t="s">
+        <v>203</v>
+      </c>
+      <c r="J29" t="s">
+        <v>203</v>
+      </c>
+      <c r="K29" t="s">
+        <v>203</v>
+      </c>
+      <c r="L29" t="s">
+        <v>203</v>
+      </c>
+      <c r="M29" t="s">
+        <v>203</v>
+      </c>
+      <c r="N29" t="s">
+        <v>203</v>
+      </c>
+      <c r="O29" t="s">
+        <v>203</v>
+      </c>
+      <c r="P29" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D33" s="9"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C20:Q26">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3176,7 +3135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4700,10 +4659,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B188"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -6221,768 +6180,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M37"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G2" t="s">
-        <v>233</v>
-      </c>
-      <c r="H2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J2" t="s">
-        <v>206</v>
-      </c>
-      <c r="K2" t="s">
-        <v>235</v>
-      </c>
-      <c r="L2" t="s">
-        <v>208</v>
-      </c>
-      <c r="M2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G3" t="s">
-        <v>233</v>
-      </c>
-      <c r="H3" t="s">
-        <v>206</v>
-      </c>
-      <c r="I3" t="s">
-        <v>234</v>
-      </c>
-      <c r="J3" t="s">
-        <v>206</v>
-      </c>
-      <c r="K3" t="s">
-        <v>235</v>
-      </c>
-      <c r="L3" t="s">
-        <v>208</v>
-      </c>
-      <c r="M3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C4" t="s">
-        <v>206</v>
-      </c>
-      <c r="D4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E4" t="s">
-        <v>207</v>
-      </c>
-      <c r="F4" t="s">
-        <v>206</v>
-      </c>
-      <c r="G4" t="s">
-        <v>237</v>
-      </c>
-      <c r="H4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I4" t="s">
-        <v>234</v>
-      </c>
-      <c r="J4" t="s">
-        <v>206</v>
-      </c>
-      <c r="K4" t="s">
-        <v>235</v>
-      </c>
-      <c r="L4" t="s">
-        <v>208</v>
-      </c>
-      <c r="M4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E5" t="s">
-        <v>207</v>
-      </c>
-      <c r="F5" t="s">
-        <v>206</v>
-      </c>
-      <c r="G5" t="s">
-        <v>233</v>
-      </c>
-      <c r="H5" t="s">
-        <v>206</v>
-      </c>
-      <c r="I5" t="s">
-        <v>238</v>
-      </c>
-      <c r="J5" t="s">
-        <v>206</v>
-      </c>
-      <c r="K5" t="s">
-        <v>235</v>
-      </c>
-      <c r="L5" t="s">
-        <v>208</v>
-      </c>
-      <c r="M5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>236</v>
-      </c>
-      <c r="B6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D6" t="s">
-        <v>232</v>
-      </c>
-      <c r="E6" t="s">
-        <v>207</v>
-      </c>
-      <c r="F6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G6" t="s">
-        <v>233</v>
-      </c>
-      <c r="H6" t="s">
-        <v>206</v>
-      </c>
-      <c r="I6" t="s">
-        <v>234</v>
-      </c>
-      <c r="J6" t="s">
-        <v>206</v>
-      </c>
-      <c r="K6" t="s">
-        <v>239</v>
-      </c>
-      <c r="L6" t="s">
-        <v>208</v>
-      </c>
-      <c r="M6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" t="s">
-        <v>205</v>
-      </c>
-      <c r="C7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D7" t="s">
-        <v>232</v>
-      </c>
-      <c r="E7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F7" t="s">
-        <v>206</v>
-      </c>
-      <c r="G7" t="s">
-        <v>237</v>
-      </c>
-      <c r="H7" t="s">
-        <v>206</v>
-      </c>
-      <c r="I7" t="s">
-        <v>234</v>
-      </c>
-      <c r="J7" t="s">
-        <v>206</v>
-      </c>
-      <c r="K7" t="s">
-        <v>235</v>
-      </c>
-      <c r="L7" t="s">
-        <v>208</v>
-      </c>
-      <c r="M7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>236</v>
-      </c>
-      <c r="B8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F8" t="s">
-        <v>206</v>
-      </c>
-      <c r="G8" t="s">
-        <v>233</v>
-      </c>
-      <c r="H8" t="s">
-        <v>206</v>
-      </c>
-      <c r="I8" t="s">
-        <v>238</v>
-      </c>
-      <c r="J8" t="s">
-        <v>206</v>
-      </c>
-      <c r="K8" t="s">
-        <v>235</v>
-      </c>
-      <c r="L8" t="s">
-        <v>208</v>
-      </c>
-      <c r="M8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>236</v>
-      </c>
-      <c r="B9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C9" t="s">
-        <v>206</v>
-      </c>
-      <c r="D9" t="s">
-        <v>232</v>
-      </c>
-      <c r="E9" t="s">
-        <v>205</v>
-      </c>
-      <c r="F9" t="s">
-        <v>206</v>
-      </c>
-      <c r="G9" t="s">
-        <v>233</v>
-      </c>
-      <c r="H9" t="s">
-        <v>206</v>
-      </c>
-      <c r="I9" t="s">
-        <v>234</v>
-      </c>
-      <c r="J9" t="s">
-        <v>206</v>
-      </c>
-      <c r="K9" t="s">
-        <v>239</v>
-      </c>
-      <c r="L9" t="s">
-        <v>208</v>
-      </c>
-      <c r="M9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>236</v>
-      </c>
-      <c r="B10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D10" t="s">
-        <v>232</v>
-      </c>
-      <c r="E10" t="s">
-        <v>207</v>
-      </c>
-      <c r="F10" t="s">
-        <v>206</v>
-      </c>
-      <c r="G10" t="s">
-        <v>237</v>
-      </c>
-      <c r="H10" t="s">
-        <v>206</v>
-      </c>
-      <c r="I10" t="s">
-        <v>238</v>
-      </c>
-      <c r="J10" t="s">
-        <v>206</v>
-      </c>
-      <c r="K10" t="s">
-        <v>235</v>
-      </c>
-      <c r="L10" t="s">
-        <v>208</v>
-      </c>
-      <c r="M10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B11" t="s">
-        <v>205</v>
-      </c>
-      <c r="C11" t="s">
-        <v>206</v>
-      </c>
-      <c r="D11" t="s">
-        <v>232</v>
-      </c>
-      <c r="E11" t="s">
-        <v>207</v>
-      </c>
-      <c r="F11" t="s">
-        <v>206</v>
-      </c>
-      <c r="G11" t="s">
-        <v>237</v>
-      </c>
-      <c r="H11" t="s">
-        <v>206</v>
-      </c>
-      <c r="I11" t="s">
-        <v>234</v>
-      </c>
-      <c r="J11" t="s">
-        <v>206</v>
-      </c>
-      <c r="K11" t="s">
-        <v>240</v>
-      </c>
-      <c r="L11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>236</v>
-      </c>
-      <c r="B12" t="s">
-        <v>205</v>
-      </c>
-      <c r="C12" t="s">
-        <v>206</v>
-      </c>
-      <c r="D12" t="s">
-        <v>232</v>
-      </c>
-      <c r="E12" t="s">
-        <v>207</v>
-      </c>
-      <c r="F12" t="s">
-        <v>206</v>
-      </c>
-      <c r="G12" t="s">
-        <v>233</v>
-      </c>
-      <c r="H12" t="s">
-        <v>206</v>
-      </c>
-      <c r="I12" t="s">
-        <v>238</v>
-      </c>
-      <c r="J12" t="s">
-        <v>206</v>
-      </c>
-      <c r="K12" t="s">
-        <v>239</v>
-      </c>
-      <c r="L12" t="s">
-        <v>208</v>
-      </c>
-      <c r="M12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>236</v>
-      </c>
-      <c r="B13" t="s">
-        <v>205</v>
-      </c>
-      <c r="C13" t="s">
-        <v>206</v>
-      </c>
-      <c r="D13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E13" t="s">
-        <v>205</v>
-      </c>
-      <c r="F13" t="s">
-        <v>206</v>
-      </c>
-      <c r="G13" t="s">
-        <v>237</v>
-      </c>
-      <c r="H13" t="s">
-        <v>206</v>
-      </c>
-      <c r="I13" t="s">
-        <v>238</v>
-      </c>
-      <c r="J13" t="s">
-        <v>206</v>
-      </c>
-      <c r="K13" t="s">
-        <v>235</v>
-      </c>
-      <c r="L13" t="s">
-        <v>208</v>
-      </c>
-      <c r="M13" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>236</v>
-      </c>
-      <c r="B14" t="s">
-        <v>205</v>
-      </c>
-      <c r="C14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" t="s">
-        <v>232</v>
-      </c>
-      <c r="E14" t="s">
-        <v>205</v>
-      </c>
-      <c r="F14" t="s">
-        <v>206</v>
-      </c>
-      <c r="G14" t="s">
-        <v>237</v>
-      </c>
-      <c r="H14" t="s">
-        <v>206</v>
-      </c>
-      <c r="I14" t="s">
-        <v>234</v>
-      </c>
-      <c r="J14" t="s">
-        <v>206</v>
-      </c>
-      <c r="K14" t="s">
-        <v>240</v>
-      </c>
-      <c r="L14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>236</v>
-      </c>
-      <c r="B15" t="s">
-        <v>205</v>
-      </c>
-      <c r="C15" t="s">
-        <v>206</v>
-      </c>
-      <c r="D15" t="s">
-        <v>232</v>
-      </c>
-      <c r="E15" t="s">
-        <v>205</v>
-      </c>
-      <c r="F15" t="s">
-        <v>206</v>
-      </c>
-      <c r="G15" t="s">
-        <v>233</v>
-      </c>
-      <c r="H15" t="s">
-        <v>206</v>
-      </c>
-      <c r="I15" t="s">
-        <v>238</v>
-      </c>
-      <c r="J15" t="s">
-        <v>206</v>
-      </c>
-      <c r="K15" t="s">
-        <v>240</v>
-      </c>
-      <c r="L15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>236</v>
-      </c>
-      <c r="B16" t="s">
-        <v>205</v>
-      </c>
-      <c r="C16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D16" t="s">
-        <v>232</v>
-      </c>
-      <c r="E16" t="s">
-        <v>207</v>
-      </c>
-      <c r="F16" t="s">
-        <v>206</v>
-      </c>
-      <c r="G16" t="s">
-        <v>237</v>
-      </c>
-      <c r="H16" t="s">
-        <v>206</v>
-      </c>
-      <c r="I16" t="s">
-        <v>238</v>
-      </c>
-      <c r="J16" t="s">
-        <v>206</v>
-      </c>
-      <c r="K16" t="s">
-        <v>240</v>
-      </c>
-      <c r="L16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>236</v>
-      </c>
-      <c r="B17" t="s">
-        <v>205</v>
-      </c>
-      <c r="C17" t="s">
-        <v>206</v>
-      </c>
-      <c r="D17" t="s">
-        <v>232</v>
-      </c>
-      <c r="E17" t="s">
-        <v>205</v>
-      </c>
-      <c r="F17" t="s">
-        <v>206</v>
-      </c>
-      <c r="G17" t="s">
-        <v>237</v>
-      </c>
-      <c r="H17" t="s">
-        <v>206</v>
-      </c>
-      <c r="I17" t="s">
-        <v>238</v>
-      </c>
-      <c r="J17" t="s">
-        <v>206</v>
-      </c>
-      <c r="K17" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>210</v>
-      </c>
-      <c r="B20" t="s">
-        <v>211</v>
-      </c>
-      <c r="C20" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>242</v>
-      </c>
-      <c r="B37" t="s">
-        <v>211</v>
-      </c>
-      <c r="C37" t="s">
-        <v>228</v>
-      </c>
-      <c r="D37" t="s">
-        <v>229</v>
-      </c>
-      <c r="E37" t="s">
-        <v>230</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>